<commit_message>
modify: 1. 在part 1的1.3末尾加了混合OLS，并把结果输出到output/part1的1.3 mix_ols_summary1.html和1.3 mix_ols_summary1.html 2. part 2里面，1.5和1.5的标题名改了下，把panel regression改成混合OLS 3. part 2的1.4和2.4加上了常数项和dummy的交乘项
</commit_message>
<xml_diff>
--- a/output/part2/January Anomaly Fama-Macbeth with time-fixed effects all months.xlsx
+++ b/output/part2/January Anomaly Fama-Macbeth with time-fixed effects all months.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,206 +462,225 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02811086389358671</v>
+        <v>0.02963681848556416</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01817035101582979</v>
+        <v>0.01814905270938225</v>
       </c>
       <c r="D2" t="n">
-        <v>1.547073244160053</v>
+        <v>1.632967789566408</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1230480230283067</v>
+        <v>0.1036723649356633</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>SMB_loading</t>
+          <t>JAN t+1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003031933021042318</v>
+        <v>0.01826231019968784</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001597272603879544</v>
+        <v>0.0155582838208262</v>
       </c>
       <c r="D3" t="n">
-        <v>1.898193842227176</v>
+        <v>1.173799784732172</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0587653256778117</v>
+        <v>0.2415370822754689</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>HML_loading</t>
+          <t>SMB_loading</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0007027159044427426</v>
+        <v>0.003171075620851749</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0009788496405509044</v>
+        <v>0.001615447416179446</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7178997420352001</v>
+        <v>1.962970499127346</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4734563082155102</v>
+        <v>0.05070345951672352</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>RMW_loading</t>
+          <t>HML_loading</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0001790579537751463</v>
+        <v>0.0006577907896868769</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001683854662385629</v>
+        <v>0.0009707244012964668</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1063381286847304</v>
+        <v>0.6776287778573956</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9153951455386933</v>
+        <v>0.4986027694196633</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>CMA_loading</t>
+          <t>RMW_loading</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0005203780283020951</v>
+        <v>-9.124669264801628e-05</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001009135935822243</v>
+        <v>0.001682365601839705</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5156669283391357</v>
+        <v>-0.05423713641567324</v>
       </c>
       <c r="E6" t="n">
-        <v>0.606520263299045</v>
+        <v>0.9567874101992</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>mkt_loading</t>
+          <t>CMA_loading</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.0003227932296571265</v>
+        <v>-0.0005290258431414854</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001420590837215257</v>
+        <v>0.001009039239031843</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.227224631611653</v>
+        <v>-0.5242866904255152</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8204256043909087</v>
+        <v>0.6005207337994569</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>size*JAN_loading</t>
+          <t>mkt_loading</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01920102260604396</v>
+        <v>-0.0003026426544363091</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5472272993005752</v>
+        <v>0.001416311050514604</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03508783759616024</v>
+        <v>-0.2136837485849925</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9720363154830455</v>
+        <v>0.8309592460526546</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BM*JAN_loading</t>
+          <t>size*JAN_loading</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5861502318089388</v>
+        <v>-0.007307766519562536</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4970317521738208</v>
+        <v>0.54696310770923</v>
       </c>
       <c r="D9" t="n">
-        <v>1.179301381139835</v>
+        <v>-0.01336062051820761</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2393439044077845</v>
+        <v>0.9893502136755956</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ROE*JAN_loading</t>
+          <t>BM*JAN_loading</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.000217756046281791</v>
+        <v>0.538102921313061</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002279924760381398</v>
+        <v>0.4995949554749016</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.09551018966317273</v>
+        <v>1.0770783720215</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9239823295289599</v>
+        <v>0.2824322186534419</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>INV*JAN_loading</t>
+          <t>ROE*JAN_loading</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0009269743769403329</v>
+        <v>-0.0001979432691203469</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002074203740144569</v>
+        <v>0.002290959030434774</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4469061351107794</v>
+        <v>-0.0864019244738661</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6553106307335861</v>
+        <v>0.931212659957</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>INV*JAN_loading</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0009285788881154748</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.002120422863847711</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.4379215598677705</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6618025878139184</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
           <t>mkt_risk_premium*JAN_loading</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>-0.2494564951270054</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.2969532082395439</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-0.8400532077288615</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.4016415647868548</v>
+      <c r="B13" t="n">
+        <v>-0.2109742443719655</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.296482670251288</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.7115904757372542</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.4773490894200991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>